<commit_message>
ADDED demo results files
</commit_message>
<xml_diff>
--- a/demo/Chocolate/Distance/Anova.xlsx
+++ b/demo/Chocolate/Distance/Anova.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Term</t>
   </si>
@@ -51,7 +51,7 @@
     <t>very large</t>
   </si>
   <si>
-    <t>small to medium</t>
+    <t>small</t>
   </si>
   <si>
     <t>very large</t>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>significance</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>**</t>
   </si>
   <si>
     <t>***</t>
@@ -116,9 +122,9 @@
     <col min="2" max="2" width="4.42578125" customWidth="true"/>
     <col min="3" max="3" width="4.42578125" customWidth="true"/>
     <col min="4" max="4" width="11.7109375" customWidth="true"/>
-    <col min="5" max="5" width="15.7109375" customWidth="true"/>
+    <col min="5" max="5" width="14.7109375" customWidth="true"/>
     <col min="6" max="6" width="13.7109375" customWidth="true"/>
-    <col min="7" max="7" width="16" customWidth="true"/>
+    <col min="7" max="7" width="10" customWidth="true"/>
     <col min="8" max="8" width="11.5703125" customWidth="true"/>
   </cols>
   <sheetData>
@@ -156,16 +162,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="0">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="D2" s="0">
-        <v>87383.061528824663</v>
+        <v>94443.533905760924</v>
       </c>
       <c r="E2" s="0">
         <v>0</v>
       </c>
       <c r="F2" s="0">
-        <v>0.9943558796444667</v>
+        <v>0.99483849405114932</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>11</v>
@@ -182,22 +188,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="0">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="D3" s="0">
-        <v>12.007677024048517</v>
+        <v>10.471349452636249</v>
       </c>
       <c r="E3" s="0">
-        <v>0.00057577695320254474</v>
+        <v>0.0012944081158074994</v>
       </c>
       <c r="F3" s="0">
-        <v>0.023636802290844292</v>
+        <v>0.020922974839795976</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -208,22 +214,22 @@
         <v>1</v>
       </c>
       <c r="C4" s="0">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="D4" s="0">
-        <v>846.84613697477539</v>
+        <v>900.1929335880933</v>
       </c>
       <c r="E4" s="0">
         <v>0</v>
       </c>
       <c r="F4" s="0">
-        <v>0.63063527060709179</v>
+        <v>0.64753093749706525</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
@@ -234,22 +240,22 @@
         <v>1</v>
       </c>
       <c r="C5" s="0">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="D5" s="0">
-        <v>146.89494053395035</v>
+        <v>147.36831823318715</v>
       </c>
       <c r="E5" s="0">
         <v>0</v>
       </c>
       <c r="F5" s="0">
-        <v>0.22848980645569886</v>
+        <v>0.23121374881277212</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>